<commit_message>
Submitted to IWSC 2020
</commit_message>
<xml_diff>
--- a/calculate_cochange/generated_csv/avg_line_coverage.xlsx
+++ b/calculate_cochange/generated_csv/avg_line_coverage.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MD NADIM\calculate_cochange\generated_csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_USASK\Programming@USASK\FindCochangeByClone\calculate_cochange\generated_csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47FFB1C-8E5A-486C-8AF0-AB86ACB8D79D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD568E7B-869B-4961-A051-13CE19FDFB91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="33">
   <si>
     <t>brlcad</t>
   </si>
@@ -76,13 +76,67 @@
   </si>
   <si>
     <t>Clone Tool</t>
+  </si>
+  <si>
+    <t>Average Recall Detected Similar Cochange</t>
+  </si>
+  <si>
+    <t>Subject Systems</t>
+  </si>
+  <si>
+    <t>ConQAT</t>
+  </si>
+  <si>
+    <t>DECKARD</t>
+  </si>
+  <si>
+    <t>iClones</t>
+  </si>
+  <si>
+    <t>NiCad</t>
+  </si>
+  <si>
+    <t>SimCAD</t>
+  </si>
+  <si>
+    <t>Simian</t>
+  </si>
+  <si>
+    <t>BRLCAD</t>
+  </si>
+  <si>
+    <t>Carol</t>
+  </si>
+  <si>
+    <t>Ctags</t>
+  </si>
+  <si>
+    <t>Freecol</t>
+  </si>
+  <si>
+    <t>Jabref</t>
+  </si>
+  <si>
+    <t>jEdit</t>
+  </si>
+  <si>
+    <t>Weighted AVG Line Coverage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is no relation of line coverage with number of change fragments. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Num of Revisions </t>
+  </si>
+  <si>
+    <t>Total Similar Cochange</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +155,29 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,12 +203,50 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -147,6 +262,937 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J$11:$O$11</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>ConQAT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DECKARD</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>iClones</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>NiCad</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SimCAD</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Simian</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$12:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>13470.631425213049</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15276.220199823687</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11239.188032618278</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9874.8265515721414</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11604.931087275934</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13433.308001763149</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8659-47EB-9BCD-A9AA450AA7A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="600411888"/>
+        <c:axId val="1095749296"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="600411888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1095749296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1095749296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="600411888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D628EAAD-B16E-4C69-8FBC-3B799F64800E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -412,31 +1458,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12:O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -446,8 +1512,32 @@
       <c r="C2" s="1">
         <v>17402.97</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="14">
+        <v>2113</v>
+      </c>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -457,8 +1547,38 @@
       <c r="C3" s="1">
         <v>13227.91</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="14">
+        <v>2113</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="1">
+        <v>2113</v>
+      </c>
+      <c r="I3" s="1">
+        <v>13821</v>
+      </c>
+      <c r="J3" s="1">
+        <v>17402.97</v>
+      </c>
+      <c r="K3" s="1">
+        <v>13227.91</v>
+      </c>
+      <c r="L3" s="1">
+        <v>14242.06</v>
+      </c>
+      <c r="M3" s="1">
+        <v>9890.7099999999991</v>
+      </c>
+      <c r="N3" s="1">
+        <v>13069.17</v>
+      </c>
+      <c r="O3" s="1">
+        <v>14129.27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -468,8 +1588,38 @@
       <c r="C4" s="1">
         <v>14242.06</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="14">
+        <v>2113</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1171</v>
+      </c>
+      <c r="I4" s="1">
+        <v>69454</v>
+      </c>
+      <c r="J4" s="1">
+        <v>4106.8500000000004</v>
+      </c>
+      <c r="K4" s="1">
+        <v>9675.2099999999991</v>
+      </c>
+      <c r="L4" s="1">
+        <v>2544.5</v>
+      </c>
+      <c r="M4" s="1">
+        <v>3714.07</v>
+      </c>
+      <c r="N4" s="1">
+        <v>5351.29</v>
+      </c>
+      <c r="O4" s="1">
+        <v>3510.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -479,8 +1629,38 @@
       <c r="C5" s="1">
         <v>9890.7099999999991</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="14">
+        <v>2114</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="1">
+        <v>773</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1963</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1697.44</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1580.44</v>
+      </c>
+      <c r="L5" s="1">
+        <v>584.85</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1863.17</v>
+      </c>
+      <c r="N5" s="1">
+        <v>721.5</v>
+      </c>
+      <c r="O5" s="1">
+        <v>746.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -490,8 +1670,38 @@
       <c r="C6" s="1">
         <v>13069.17</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="14">
+        <v>2112</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1001</v>
+      </c>
+      <c r="I6" s="1">
+        <v>246083</v>
+      </c>
+      <c r="J6" s="1">
+        <v>10446.49</v>
+      </c>
+      <c r="K6" s="1">
+        <v>19891.580000000002</v>
+      </c>
+      <c r="L6" s="1">
+        <v>5229.6400000000003</v>
+      </c>
+      <c r="M6" s="1">
+        <v>6986.84</v>
+      </c>
+      <c r="N6" s="1">
+        <v>12527.23</v>
+      </c>
+      <c r="O6" s="1">
+        <v>5507.26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -501,8 +1711,38 @@
       <c r="C7" s="1">
         <v>14129.27</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="14">
+        <v>2114</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1537</v>
+      </c>
+      <c r="I7" s="1">
+        <v>79417</v>
+      </c>
+      <c r="J7" s="1">
+        <v>7981.96</v>
+      </c>
+      <c r="K7" s="1">
+        <v>15753.07</v>
+      </c>
+      <c r="L7" s="1">
+        <v>4243</v>
+      </c>
+      <c r="M7" s="1">
+        <v>4341.7700000000004</v>
+      </c>
+      <c r="N7" s="1">
+        <v>6975.55</v>
+      </c>
+      <c r="O7" s="1">
+        <v>4255.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -512,8 +1752,38 @@
       <c r="C8" s="1">
         <v>4106.8500000000004</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="14">
+        <v>1173</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="1">
+        <v>211</v>
+      </c>
+      <c r="I8" s="1">
+        <v>160689</v>
+      </c>
+      <c r="J8" s="1">
+        <v>123517.49</v>
+      </c>
+      <c r="K8" s="1">
+        <v>91678.15</v>
+      </c>
+      <c r="L8" s="1">
+        <v>147925.98000000001</v>
+      </c>
+      <c r="M8" s="1">
+        <v>127262.87</v>
+      </c>
+      <c r="N8" s="1">
+        <v>100866.1</v>
+      </c>
+      <c r="O8" s="1">
+        <v>212471.21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -523,8 +1793,35 @@
       <c r="C9" s="1">
         <v>9675.2099999999991</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="14">
+        <v>1173</v>
+      </c>
+      <c r="J9" s="4">
+        <f>AVERAGE(J3:J8)</f>
+        <v>27525.533333333336</v>
+      </c>
+      <c r="K9" s="4">
+        <f t="shared" ref="K9:O9" si="0">AVERAGE(K3:K8)</f>
+        <v>25301.059999999998</v>
+      </c>
+      <c r="L9" s="4">
+        <f t="shared" si="0"/>
+        <v>29128.338333333333</v>
+      </c>
+      <c r="M9" s="4">
+        <f t="shared" si="0"/>
+        <v>25676.571666666667</v>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="0"/>
+        <v>23251.806666666667</v>
+      </c>
+      <c r="O9" s="4">
+        <f>AVERAGE(O3:O8)</f>
+        <v>40103.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -534,8 +1831,11 @@
       <c r="C10" s="1">
         <v>2544.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="14">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -545,8 +1845,40 @@
       <c r="C11" s="1">
         <v>3714.07</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="14">
+        <v>1166</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="P11" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -556,8 +1888,46 @@
       <c r="C12" s="1">
         <v>5351.29</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="14">
+        <v>1173</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="9">
+        <f>((J3*H3)+(J4*H4)+(J5*H5)+(J6*H6)+(J7*H7)+(J8*H8))/(H3+H4+H5+H6+H7+H8)</f>
+        <v>13470.631425213049</v>
+      </c>
+      <c r="K12" s="9">
+        <f>((K3*H3)+(K4*H4)+(K5*H5)+(K6*H6)+(K7*H7)+(K8*H8))/(H3+H4+H5+H6+H7+H8)</f>
+        <v>15276.220199823687</v>
+      </c>
+      <c r="L12" s="9">
+        <f>((L3*H3)+(L4*H4)+(L5*H5)+(L6*H6)+(L7*H7)+(L8*H8))/(H3+H4+H5+H6+H7+H8)</f>
+        <v>11239.188032618278</v>
+      </c>
+      <c r="M12" s="9">
+        <f>((M3*H3)+(M4*H4)+(M5*H5)+(M6*H6)+(M7*H7)+(M8*H8))/(H3+H4+H5+H6+H7+H8)</f>
+        <v>9874.8265515721414</v>
+      </c>
+      <c r="N12" s="9">
+        <f>((N3*H3)+(N4*H4)+(N5*H5)+(N6*H6)+(N7*H7)+(N8*H8))/(H3+H4+H5+H6+H7+H8)</f>
+        <v>11604.931087275934</v>
+      </c>
+      <c r="O12" s="9">
+        <f>((O3*H3)+(O4*H4)+(O5*H5)+(O6*H6)+(O7*H7)+(O8*H8))/(H3+H4+H5+H6+H7+H8)</f>
+        <v>13433.308001763149</v>
+      </c>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -567,8 +1937,11 @@
       <c r="C13" s="1">
         <v>3510.05</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="14">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -578,8 +1951,11 @@
       <c r="C14" s="1">
         <v>1697.44</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="14">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -589,8 +1965,19 @@
       <c r="C15" s="1">
         <v>1580.44</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="14">
+        <v>773</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -600,8 +1987,19 @@
       <c r="C16" s="1">
         <v>584.85</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="14">
+        <v>773</v>
+      </c>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -611,8 +2009,31 @@
       <c r="C17" s="1">
         <v>1863.17</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="14">
+        <v>770</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="11"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -622,8 +2043,31 @@
       <c r="C18" s="1">
         <v>721.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="14">
+        <v>741</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="13">
+        <v>27525.53</v>
+      </c>
+      <c r="H18" s="13">
+        <v>25301.06</v>
+      </c>
+      <c r="I18" s="13">
+        <v>29128.34</v>
+      </c>
+      <c r="J18" s="13">
+        <v>25676.57</v>
+      </c>
+      <c r="K18" s="13">
+        <v>23251.81</v>
+      </c>
+      <c r="L18" s="13">
+        <v>40103.25</v>
+      </c>
+      <c r="M18" s="11"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -633,8 +2077,19 @@
       <c r="C19" s="1">
         <v>746.26</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="14">
+        <v>617</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -644,8 +2099,19 @@
       <c r="C20" s="1">
         <v>10446.49</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="14">
+        <v>1001</v>
+      </c>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -655,8 +2121,19 @@
       <c r="C21" s="1">
         <v>19891.580000000002</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="14">
+        <v>1001</v>
+      </c>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -666,8 +2143,23 @@
       <c r="C22" s="1">
         <v>5229.6400000000003</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="14">
+        <v>1001</v>
+      </c>
+      <c r="F22" s="11"/>
+      <c r="G22" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="13">
+        <v>26993.87</v>
+      </c>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -677,8 +2169,23 @@
       <c r="C23" s="1">
         <v>6986.84</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="14">
+        <v>1001</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="13">
+        <v>27535.56</v>
+      </c>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -688,8 +2195,23 @@
       <c r="C24" s="1">
         <v>12527.23</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="14">
+        <v>1001</v>
+      </c>
+      <c r="F24" s="11"/>
+      <c r="G24" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="13">
+        <v>27595.48</v>
+      </c>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -699,8 +2221,23 @@
       <c r="C25" s="1">
         <v>5507.26</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="14">
+        <v>1001</v>
+      </c>
+      <c r="F25" s="11"/>
+      <c r="G25" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="13">
+        <v>24765.71</v>
+      </c>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -710,8 +2247,23 @@
       <c r="C26" s="1">
         <v>7981.96</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="14">
+        <v>1538</v>
+      </c>
+      <c r="F26" s="11"/>
+      <c r="G26" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="13">
+        <v>23631.06</v>
+      </c>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -721,8 +2273,23 @@
       <c r="C27" s="1">
         <v>15753.07</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="14">
+        <v>1540</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="13">
+        <v>37904.269999999997</v>
+      </c>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -732,8 +2299,11 @@
       <c r="C28" s="1">
         <v>4243</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="14">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -743,8 +2313,11 @@
       <c r="C29" s="1">
         <v>4341.7700000000004</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="14">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -754,8 +2327,11 @@
       <c r="C30" s="1">
         <v>6975.55</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="14">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -765,8 +2341,11 @@
       <c r="C31" s="1">
         <v>4255.45</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="14">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -776,8 +2355,11 @@
       <c r="C32" s="1">
         <v>123517.49</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="14">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -787,8 +2369,11 @@
       <c r="C33" s="1">
         <v>91678.15</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="14">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -798,8 +2383,11 @@
       <c r="C34" s="1">
         <v>147925.98000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="14">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -809,8 +2397,11 @@
       <c r="C35" s="1">
         <v>127262.87</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="14">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -820,8 +2411,11 @@
       <c r="C36" s="1">
         <v>100866.1</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="14">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -831,8 +2425,21 @@
       <c r="C37" s="1">
         <v>212471.21</v>
       </c>
+      <c r="D37" s="14">
+        <v>211</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="P11:U12"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="G1:G2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>